<commit_message>
fix: arregle los shapefiles de guatemala para que tubieran el código departamental y asi estandarizar el codigo. Siempre es necesario tener el geocodigo departamental y municipal.
</commit_message>
<xml_diff>
--- a/src/Shapefile_prep/shapefile_settings.xlsx
+++ b/src/Shapefile_prep/shapefile_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisfernandoquezada/Documents/GitHub/omrat/src/Shapefile_prep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/Shapefile_prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87E397F-FA4A-B34C-A51B-88221FFAFB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503F6BB3-6E37-A841-996B-05CB71A95EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="19380" xr2:uid="{9BCEFF0F-9A23-954A-B88D-C463C9BBC742}"/>
+    <workbookView xWindow="3780" yWindow="760" windowWidth="17920" windowHeight="18880" xr2:uid="{9BCEFF0F-9A23-954A-B88D-C463C9BBC742}"/>
   </bookViews>
   <sheets>
     <sheet name="SETTINGS" sheetId="2" r:id="rId1"/>
@@ -68,19 +68,19 @@
     <t>ADMIN1 ID</t>
   </si>
   <si>
-    <t>PROV_CODE</t>
-  </si>
-  <si>
-    <t>PROVINCIA</t>
-  </si>
-  <si>
-    <t>MUNI_CODE</t>
-  </si>
-  <si>
-    <t>MUNICIPIO</t>
-  </si>
-  <si>
-    <t>DR_Municipios</t>
+    <t>guatemala</t>
+  </si>
+  <si>
+    <t>ADMIN1G</t>
+  </si>
+  <si>
+    <t>ADMIN1</t>
+  </si>
+  <si>
+    <t>GEO_ID</t>
+  </si>
+  <si>
+    <t>ADMIN2</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -568,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -586,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2"/>
     </row>

</xml_diff>